<commit_message>
Tests angepasst. Alle Tests laufen.
</commit_message>
<xml_diff>
--- a/src/main/4 neuen Mitarbeiter anlegen/1 Mitarbeiter.xlsx
+++ b/src/main/4 neuen Mitarbeiter anlegen/1 Mitarbeiter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\4 neuen Mitarbeiter anlegen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30CDA5F-63D1-438E-86A5-1CDCD38D10E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6749D32D-223A-4227-A183-813E81C0189F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1548" yWindow="2196" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="87">
   <si>
     <t>11 111 111 111</t>
   </si>
@@ -154,9 +154,6 @@
     <t>Zuschuss private Krankenversicherung</t>
   </si>
   <si>
-    <t>wohnhaft Sachsen?</t>
-  </si>
-  <si>
     <t>Tarifbeschaeftigt?</t>
   </si>
   <si>
@@ -284,6 +281,12 @@
   </si>
   <si>
     <t>juenger als 23 oder vor 1940 geboren?</t>
+  </si>
+  <si>
+    <t>zahlt AN-Minijob-Rentenpauschale</t>
+  </si>
+  <si>
+    <t>AG-Standort in Sachsen?</t>
   </si>
 </sst>
 </file>
@@ -329,7 +332,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -366,12 +369,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -385,6 +397,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -789,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:B41"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -814,7 +828,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -822,7 +836,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -836,7 +850,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -913,10 +927,10 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -945,10 +959,10 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -956,7 +970,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -964,7 +978,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -980,7 +994,7 @@
         <v>32</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -988,7 +1002,7 @@
         <v>33</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -1012,23 +1026,23 @@
         <v>37</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -1036,7 +1050,7 @@
         <v>35</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -1044,7 +1058,7 @@
         <v>36</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1052,15 +1066,15 @@
         <v>34</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1068,52 +1082,52 @@
         <v>40</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B40" s="10">
         <v>1</v>
@@ -1121,74 +1135,78 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="4">
-        <v>0</v>
-      </c>
+      <c r="B44" s="4"/>
     </row>
     <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>78</v>
-      </c>
-      <c r="B45" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" s="4"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B46" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="7" t="s">
+      <c r="B48" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B48" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>52</v>
+      <c r="B50" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1223,7 +1241,7 @@
           <x14:formula1>
             <xm:f>Tabelle2!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B29 B38:B39 B35 B46:B49 B42:B43 B33 B41</xm:sqref>
+          <xm:sqref>B29 B38:B39 B35 B46:B50 B42:B43 B33 B41</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BC540D61-4588-479B-B62B-BA6755FB2963}">
           <x14:formula1>
@@ -1267,52 +1285,52 @@
         <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1321,7 +1339,7 @@
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Erstellung der endgueltigen Ordnerstruktur
</commit_message>
<xml_diff>
--- a/src/main/4 neuen Mitarbeiter anlegen/1 Mitarbeiter.xlsx
+++ b/src/main/4 neuen Mitarbeiter anlegen/1 Mitarbeiter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\4 neuen Mitarbeiter anlegen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6749D32D-223A-4227-A183-813E81C0189F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDBAAEB-852D-4DC6-9AA6-FBFD67CE43C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1548" yWindow="2196" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1146,7 +1146,7 @@
         <v>86</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>